<commit_message>
Further work on v6.6:  Added CalibrateMode SoilWater outputs for Paul Henne.  Enabled CSV input for FunctionalGroupParameters.  Tested.  Updated documentation.
</commit_message>
<xml_diff>
--- a/testing/Core7-NECN6.6/NECN_Spp_Table.xlsx
+++ b/testing/Core7-NECN6.6/NECN_Spp_Table.xlsx
@@ -29,9 +29,6 @@
     <t>SpeciesCode</t>
   </si>
   <si>
-    <t>FunctionalType</t>
-  </si>
-  <si>
     <t>NitrogenFixer</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>FixnSeed</t>
+  </si>
+  <si>
+    <t>FunctionalGroupIndex</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:AB1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,66 +456,66 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>3</v>

</xml_diff>